<commit_message>
added write_total_takes and write_partial_takes(wip)
</commit_message>
<xml_diff>
--- a/grafic_output.xlsx
+++ b/grafic_output.xlsx
@@ -1979,12 +1979,16 @@
       </c>
     </row>
     <row r="8" ht="13.75" customHeight="1" s="19">
-      <c r="A8" s="41" t="n"/>
-      <c r="B8" s="24" t="n"/>
+      <c r="A8" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C8" s="25" t="n"/>
       <c r="D8" s="26" t="inlineStr">
         <is>
-          <t>NIÑERA</t>
+          <t>HOMBRE 3</t>
         </is>
       </c>
       <c r="E8" s="27" t="n"/>
@@ -2039,12 +2043,16 @@
       <c r="BB8" s="32" t="n"/>
     </row>
     <row r="9" ht="13.75" customHeight="1" s="19">
-      <c r="A9" s="41" t="n"/>
-      <c r="B9" s="24" t="n"/>
+      <c r="A9" s="41" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C9" s="25" t="n"/>
       <c r="D9" s="26" t="inlineStr">
         <is>
-          <t>HANNA</t>
+          <t>INSERTO</t>
         </is>
       </c>
       <c r="E9" s="27" t="n"/>
@@ -2099,12 +2107,16 @@
       <c r="BB9" s="33" t="n"/>
     </row>
     <row r="10" ht="13.75" customHeight="1" s="19">
-      <c r="A10" s="41" t="n"/>
-      <c r="B10" s="24" t="n"/>
+      <c r="A10" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C10" s="25" t="n"/>
       <c r="D10" s="26" t="inlineStr">
         <is>
-          <t>LUCIO</t>
+          <t>MUJER</t>
         </is>
       </c>
       <c r="E10" s="27" t="n"/>
@@ -2159,12 +2171,16 @@
       <c r="BB10" s="33" t="n"/>
     </row>
     <row r="11" ht="13.75" customHeight="1" s="19">
-      <c r="A11" s="41" t="n"/>
-      <c r="B11" s="24" t="n"/>
+      <c r="A11" s="41" t="n">
+        <v>26</v>
+      </c>
+      <c r="B11" s="24" t="n">
+        <v>8</v>
+      </c>
       <c r="C11" s="25" t="n"/>
       <c r="D11" s="26" t="inlineStr">
         <is>
-          <t>MUJER</t>
+          <t>IDA</t>
         </is>
       </c>
       <c r="E11" s="27" t="n"/>
@@ -2219,12 +2235,16 @@
       <c r="BB11" s="33" t="n"/>
     </row>
     <row r="12" ht="13.75" customHeight="1" s="19">
-      <c r="A12" s="41" t="n"/>
-      <c r="B12" s="24" t="n"/>
+      <c r="A12" s="41" t="n">
+        <v>14</v>
+      </c>
+      <c r="B12" s="24" t="n">
+        <v>5</v>
+      </c>
       <c r="C12" s="25" t="n"/>
       <c r="D12" s="26" t="inlineStr">
         <is>
-          <t>IDA</t>
+          <t>ANTON</t>
         </is>
       </c>
       <c r="E12" s="27" t="n"/>
@@ -2279,12 +2299,16 @@
       <c r="BB12" s="33" t="n"/>
     </row>
     <row r="13" ht="13.75" customHeight="1" s="19">
-      <c r="A13" s="41" t="n"/>
-      <c r="B13" s="24" t="n"/>
+      <c r="A13" s="41" t="n">
+        <v>106</v>
+      </c>
+      <c r="B13" s="24" t="n">
+        <v>34</v>
+      </c>
       <c r="C13" s="25" t="n"/>
       <c r="D13" s="26" t="inlineStr">
         <is>
-          <t>TÍTULO</t>
+          <t>HANNA</t>
         </is>
       </c>
       <c r="E13" s="27" t="n"/>
@@ -2339,12 +2363,16 @@
       <c r="BB13" s="33" t="n"/>
     </row>
     <row r="14" ht="13.75" customHeight="1" s="19">
-      <c r="A14" s="41" t="n"/>
-      <c r="B14" s="24" t="n"/>
+      <c r="A14" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="B14" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C14" s="25" t="n"/>
       <c r="D14" s="26" t="inlineStr">
         <is>
-          <t>ANTON</t>
+          <t>HOMBRE 1</t>
         </is>
       </c>
       <c r="E14" s="27" t="n"/>
@@ -2399,8 +2427,12 @@
       <c r="BB14" s="33" t="n"/>
     </row>
     <row r="15" ht="13.75" customHeight="1" s="19">
-      <c r="A15" s="41" t="n"/>
-      <c r="B15" s="24" t="n"/>
+      <c r="A15" s="41" t="n">
+        <v>47</v>
+      </c>
+      <c r="B15" s="24" t="n">
+        <v>16</v>
+      </c>
       <c r="C15" s="25" t="n"/>
       <c r="D15" s="26" t="inlineStr">
         <is>
@@ -2459,12 +2491,16 @@
       <c r="BB15" s="33" t="n"/>
     </row>
     <row r="16" ht="13.75" customHeight="1" s="19">
-      <c r="A16" s="41" t="n"/>
-      <c r="B16" s="24" t="n"/>
+      <c r="A16" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" s="24" t="n">
+        <v>0</v>
+      </c>
       <c r="C16" s="25" t="n"/>
       <c r="D16" s="26" t="inlineStr">
         <is>
-          <t>AMBIENTE HOMBRES</t>
+          <t>NIÑERA</t>
         </is>
       </c>
       <c r="E16" s="27" t="n"/>
@@ -2519,12 +2555,16 @@
       <c r="BB16" s="33" t="n"/>
     </row>
     <row r="17" ht="13.75" customHeight="1" s="19">
-      <c r="A17" s="41" t="n"/>
-      <c r="B17" s="24" t="n"/>
+      <c r="A17" s="41" t="n">
+        <v>5</v>
+      </c>
+      <c r="B17" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C17" s="25" t="n"/>
       <c r="D17" s="26" t="inlineStr">
         <is>
-          <t>PROFESORA</t>
+          <t>HOMBRE 2</t>
         </is>
       </c>
       <c r="E17" s="27" t="n"/>
@@ -2579,12 +2619,16 @@
       <c r="BB17" s="33" t="n"/>
     </row>
     <row r="18" ht="13.75" customHeight="1" s="19">
-      <c r="A18" s="41" t="n"/>
-      <c r="B18" s="24" t="n"/>
+      <c r="A18" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="B18" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C18" s="25" t="n"/>
       <c r="D18" s="26" t="inlineStr">
         <is>
-          <t>LOTTE</t>
+          <t>PROFESORA</t>
         </is>
       </c>
       <c r="E18" s="27" t="n"/>
@@ -2639,12 +2683,16 @@
       <c r="BB18" s="33" t="n"/>
     </row>
     <row r="19" ht="13.75" customHeight="1" s="19">
-      <c r="A19" s="41" t="n"/>
-      <c r="B19" s="24" t="n"/>
+      <c r="A19" s="41" t="n">
+        <v>5</v>
+      </c>
+      <c r="B19" s="24" t="n">
+        <v>3</v>
+      </c>
       <c r="C19" s="25" t="n"/>
       <c r="D19" s="26" t="inlineStr">
         <is>
-          <t>HOMBRE 1</t>
+          <t>MARIE</t>
         </is>
       </c>
       <c r="E19" s="27" t="n"/>
@@ -2699,12 +2747,16 @@
       <c r="BB19" s="33" t="n"/>
     </row>
     <row r="20" ht="13.75" customHeight="1" s="19">
-      <c r="A20" s="41" t="n"/>
-      <c r="B20" s="24" t="n"/>
+      <c r="A20" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C20" s="25" t="n"/>
       <c r="D20" s="26" t="inlineStr">
         <is>
-          <t>HELENE</t>
+          <t>PROFESOR</t>
         </is>
       </c>
       <c r="E20" s="27" t="n"/>
@@ -2759,12 +2811,16 @@
       <c r="BB20" s="33" t="n"/>
     </row>
     <row r="21" ht="13.75" customHeight="1" s="19">
-      <c r="A21" s="41" t="n"/>
-      <c r="B21" s="24" t="n"/>
+      <c r="A21" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" s="24" t="n">
+        <v>0</v>
+      </c>
       <c r="C21" s="25" t="n"/>
       <c r="D21" s="26" t="inlineStr">
         <is>
-          <t>HOMBRE</t>
+          <t>AMBIENTE NIÑAS</t>
         </is>
       </c>
       <c r="E21" s="27" t="n"/>
@@ -2819,12 +2875,16 @@
       <c r="BB21" s="33" t="n"/>
     </row>
     <row r="22" ht="13.75" customHeight="1" s="19">
-      <c r="A22" s="41" t="n"/>
-      <c r="B22" s="24" t="n"/>
+      <c r="A22" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="B22" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C22" s="25" t="n"/>
       <c r="D22" s="26" t="inlineStr">
         <is>
-          <t>HOMBRE 2</t>
+          <t>LISA</t>
         </is>
       </c>
       <c r="E22" s="27" t="n"/>
@@ -2879,12 +2939,16 @@
       <c r="BB22" s="33" t="n"/>
     </row>
     <row r="23" ht="13.75" customHeight="1" s="19">
-      <c r="A23" s="41" t="n"/>
-      <c r="B23" s="24" t="n"/>
+      <c r="A23" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="B23" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C23" s="25" t="n"/>
       <c r="D23" s="26" t="inlineStr">
         <is>
-          <t>HOMBRE 3</t>
+          <t>TÍTULO</t>
         </is>
       </c>
       <c r="E23" s="27" t="n"/>
@@ -2939,12 +3003,16 @@
       <c r="BB23" s="33" t="n"/>
     </row>
     <row r="24" ht="13.75" customHeight="1" s="19">
-      <c r="A24" s="41" t="n"/>
-      <c r="B24" s="24" t="n"/>
+      <c r="A24" s="41" t="n">
+        <v>6</v>
+      </c>
+      <c r="B24" s="24" t="n">
+        <v>2</v>
+      </c>
       <c r="C24" s="25" t="n"/>
       <c r="D24" s="26" t="inlineStr">
         <is>
-          <t>LISA</t>
+          <t>HELENE</t>
         </is>
       </c>
       <c r="E24" s="27" t="n"/>
@@ -2999,12 +3067,16 @@
       <c r="BB24" s="33" t="n"/>
     </row>
     <row r="25" ht="13.75" customHeight="1" s="19">
-      <c r="A25" s="41" t="n"/>
-      <c r="B25" s="24" t="n"/>
+      <c r="A25" s="41" t="n">
+        <v>16</v>
+      </c>
+      <c r="B25" s="24" t="n">
+        <v>3</v>
+      </c>
       <c r="C25" s="25" t="n"/>
       <c r="D25" s="26" t="inlineStr">
         <is>
-          <t>INSERTO</t>
+          <t>LOTTE</t>
         </is>
       </c>
       <c r="E25" s="27" t="n"/>
@@ -3059,12 +3131,16 @@
       <c r="BB25" s="33" t="n"/>
     </row>
     <row r="26" ht="13.75" customHeight="1" s="19">
-      <c r="A26" s="41" t="n"/>
-      <c r="B26" s="24" t="n"/>
+      <c r="A26" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="B26" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C26" s="30" t="n"/>
       <c r="D26" s="26" t="inlineStr">
         <is>
-          <t>AMBIENTE NIÑAS</t>
+          <t>AMBIENTE HOMBRES</t>
         </is>
       </c>
       <c r="E26" s="27" t="n"/>
@@ -3119,12 +3195,16 @@
       <c r="BB26" s="33" t="n"/>
     </row>
     <row r="27" ht="13.75" customHeight="1" s="19">
-      <c r="A27" s="41" t="n"/>
-      <c r="B27" s="24" t="n"/>
+      <c r="A27" s="41" t="n">
+        <v>4</v>
+      </c>
+      <c r="B27" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C27" s="25" t="n"/>
       <c r="D27" s="26" t="inlineStr">
         <is>
-          <t>PROFESOR</t>
+          <t>LUCIO</t>
         </is>
       </c>
       <c r="E27" s="27" t="n"/>
@@ -3179,12 +3259,16 @@
       <c r="BB27" s="33" t="n"/>
     </row>
     <row r="28" ht="13.75" customHeight="1" s="19">
-      <c r="A28" s="41" t="n"/>
-      <c r="B28" s="24" t="n"/>
+      <c r="A28" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="B28" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C28" s="25" t="n"/>
       <c r="D28" s="26" t="inlineStr">
         <is>
-          <t>AMB</t>
+          <t>HOMBRE</t>
         </is>
       </c>
       <c r="E28" s="27" t="n"/>
@@ -3239,12 +3323,16 @@
       <c r="BB28" s="33" t="n"/>
     </row>
     <row r="29" ht="13.75" customHeight="1" s="19">
-      <c r="A29" s="41" t="n"/>
-      <c r="B29" s="24" t="n"/>
+      <c r="A29" s="41" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="24" t="n">
+        <v>7</v>
+      </c>
       <c r="C29" s="25" t="n"/>
       <c r="D29" s="26" t="inlineStr">
         <is>
-          <t>MARIE</t>
+          <t>AMB</t>
         </is>
       </c>
       <c r="E29" s="27" t="n"/>
@@ -4932,12 +5020,16 @@
       </c>
     </row>
     <row r="8" ht="13.75" customHeight="1" s="19">
-      <c r="A8" s="41" t="n"/>
-      <c r="B8" s="24" t="n"/>
+      <c r="A8" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C8" s="25" t="n"/>
       <c r="D8" s="26" t="inlineStr">
         <is>
-          <t>IDA</t>
+          <t>MUJER 2</t>
         </is>
       </c>
       <c r="E8" s="27" t="n"/>
@@ -4992,12 +5084,16 @@
       <c r="BB8" s="32" t="n"/>
     </row>
     <row r="9" ht="13.75" customHeight="1" s="19">
-      <c r="A9" s="41" t="n"/>
-      <c r="B9" s="24" t="n"/>
+      <c r="A9" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C9" s="25" t="n"/>
       <c r="D9" s="26" t="inlineStr">
         <is>
-          <t>LOTTE</t>
+          <t>HOMBRE 3</t>
         </is>
       </c>
       <c r="E9" s="27" t="n"/>
@@ -5052,12 +5148,16 @@
       <c r="BB9" s="33" t="n"/>
     </row>
     <row r="10" ht="13.75" customHeight="1" s="19">
-      <c r="A10" s="41" t="n"/>
-      <c r="B10" s="24" t="n"/>
+      <c r="A10" s="41" t="n">
+        <v>5</v>
+      </c>
+      <c r="B10" s="24" t="n">
+        <v>4</v>
+      </c>
       <c r="C10" s="25" t="n"/>
       <c r="D10" s="26" t="inlineStr">
         <is>
-          <t>HOMBRES</t>
+          <t>HOMBRE 2</t>
         </is>
       </c>
       <c r="E10" s="27" t="n"/>
@@ -5112,12 +5212,16 @@
       <c r="BB10" s="33" t="n"/>
     </row>
     <row r="11" ht="13.75" customHeight="1" s="19">
-      <c r="A11" s="41" t="n"/>
-      <c r="B11" s="24" t="n"/>
+      <c r="A11" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C11" s="25" t="n"/>
       <c r="D11" s="26" t="inlineStr">
         <is>
-          <t>ANTON</t>
+          <t>AGNES</t>
         </is>
       </c>
       <c r="E11" s="27" t="n"/>
@@ -5172,12 +5276,16 @@
       <c r="BB11" s="33" t="n"/>
     </row>
     <row r="12" ht="13.75" customHeight="1" s="19">
-      <c r="A12" s="41" t="n"/>
-      <c r="B12" s="24" t="n"/>
+      <c r="A12" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C12" s="25" t="n"/>
       <c r="D12" s="26" t="inlineStr">
         <is>
-          <t>HOMBRE 1</t>
+          <t>HOMBRES</t>
         </is>
       </c>
       <c r="E12" s="27" t="n"/>
@@ -5232,12 +5340,16 @@
       <c r="BB12" s="33" t="n"/>
     </row>
     <row r="13" ht="13.75" customHeight="1" s="19">
-      <c r="A13" s="41" t="n"/>
-      <c r="B13" s="24" t="n"/>
+      <c r="A13" s="41" t="n">
+        <v>6</v>
+      </c>
+      <c r="B13" s="24" t="n">
+        <v>2</v>
+      </c>
       <c r="C13" s="25" t="n"/>
       <c r="D13" s="26" t="inlineStr">
         <is>
-          <t>HELENE</t>
+          <t>HERMANN</t>
         </is>
       </c>
       <c r="E13" s="27" t="n"/>
@@ -5292,12 +5404,16 @@
       <c r="BB13" s="33" t="n"/>
     </row>
     <row r="14" ht="13.75" customHeight="1" s="19">
-      <c r="A14" s="41" t="n"/>
-      <c r="B14" s="24" t="n"/>
+      <c r="A14" s="41" t="n">
+        <v>26</v>
+      </c>
+      <c r="B14" s="24" t="n">
+        <v>8</v>
+      </c>
       <c r="C14" s="25" t="n"/>
       <c r="D14" s="26" t="inlineStr">
         <is>
-          <t>OTTO</t>
+          <t>IDA</t>
         </is>
       </c>
       <c r="E14" s="27" t="n"/>
@@ -5352,12 +5468,16 @@
       <c r="BB14" s="33" t="n"/>
     </row>
     <row r="15" ht="13.75" customHeight="1" s="19">
-      <c r="A15" s="41" t="n"/>
-      <c r="B15" s="24" t="n"/>
+      <c r="A15" s="41" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="24" t="n">
+        <v>4</v>
+      </c>
       <c r="C15" s="25" t="n"/>
       <c r="D15" s="26" t="inlineStr">
         <is>
-          <t>HERMANN</t>
+          <t>ANTON</t>
         </is>
       </c>
       <c r="E15" s="27" t="n"/>
@@ -5412,12 +5532,16 @@
       <c r="BB15" s="33" t="n"/>
     </row>
     <row r="16" ht="13.75" customHeight="1" s="19">
-      <c r="A16" s="41" t="n"/>
-      <c r="B16" s="24" t="n"/>
+      <c r="A16" s="41" t="n">
+        <v>6</v>
+      </c>
+      <c r="B16" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C16" s="25" t="n"/>
       <c r="D16" s="26" t="inlineStr">
         <is>
-          <t>AMB</t>
+          <t>HELENE</t>
         </is>
       </c>
       <c r="E16" s="27" t="n"/>
@@ -5472,12 +5596,16 @@
       <c r="BB16" s="33" t="n"/>
     </row>
     <row r="17" ht="13.75" customHeight="1" s="19">
-      <c r="A17" s="41" t="n"/>
-      <c r="B17" s="24" t="n"/>
+      <c r="A17" s="41" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="24" t="n">
+        <v>3</v>
+      </c>
       <c r="C17" s="25" t="n"/>
       <c r="D17" s="26" t="inlineStr">
         <is>
-          <t>MUJER 2</t>
+          <t>LOTTE</t>
         </is>
       </c>
       <c r="E17" s="27" t="n"/>
@@ -5532,12 +5660,16 @@
       <c r="BB17" s="33" t="n"/>
     </row>
     <row r="18" ht="13.75" customHeight="1" s="19">
-      <c r="A18" s="41" t="n"/>
-      <c r="B18" s="24" t="n"/>
+      <c r="A18" s="41" t="n">
+        <v>106</v>
+      </c>
+      <c r="B18" s="24" t="n">
+        <v>30</v>
+      </c>
       <c r="C18" s="25" t="n"/>
       <c r="D18" s="26" t="inlineStr">
         <is>
-          <t>HOMBRE 2</t>
+          <t>HANNA</t>
         </is>
       </c>
       <c r="E18" s="27" t="n"/>
@@ -5592,12 +5724,16 @@
       <c r="BB18" s="33" t="n"/>
     </row>
     <row r="19" ht="13.75" customHeight="1" s="19">
-      <c r="A19" s="41" t="n"/>
-      <c r="B19" s="24" t="n"/>
+      <c r="A19" s="41" t="n">
+        <v>28</v>
+      </c>
+      <c r="B19" s="24" t="n">
+        <v>7</v>
+      </c>
       <c r="C19" s="25" t="n"/>
       <c r="D19" s="26" t="inlineStr">
         <is>
-          <t>HOMBRE 3</t>
+          <t>AMB</t>
         </is>
       </c>
       <c r="E19" s="27" t="n"/>
@@ -5652,12 +5788,16 @@
       <c r="BB19" s="33" t="n"/>
     </row>
     <row r="20" ht="13.75" customHeight="1" s="19">
-      <c r="A20" s="41" t="n"/>
-      <c r="B20" s="24" t="n"/>
+      <c r="A20" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="B20" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C20" s="25" t="n"/>
       <c r="D20" s="26" t="inlineStr">
         <is>
-          <t>HANNA</t>
+          <t>HOMBRE 1</t>
         </is>
       </c>
       <c r="E20" s="27" t="n"/>
@@ -5712,12 +5852,16 @@
       <c r="BB20" s="33" t="n"/>
     </row>
     <row r="21" ht="13.75" customHeight="1" s="19">
-      <c r="A21" s="41" t="n"/>
-      <c r="B21" s="24" t="n"/>
+      <c r="A21" s="41" t="n">
+        <v>47</v>
+      </c>
+      <c r="B21" s="24" t="n">
+        <v>17</v>
+      </c>
       <c r="C21" s="25" t="n"/>
       <c r="D21" s="26" t="inlineStr">
         <is>
-          <t>AGNES</t>
+          <t>OTTO</t>
         </is>
       </c>
       <c r="E21" s="27" t="n"/>
@@ -5772,8 +5916,12 @@
       <c r="BB21" s="33" t="n"/>
     </row>
     <row r="22" ht="13.75" customHeight="1" s="19">
-      <c r="A22" s="41" t="n"/>
-      <c r="B22" s="24" t="n"/>
+      <c r="A22" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="B22" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C22" s="25" t="n"/>
       <c r="D22" s="26" t="inlineStr">
         <is>
@@ -5832,12 +5980,16 @@
       <c r="BB22" s="33" t="n"/>
     </row>
     <row r="23" ht="13.75" customHeight="1" s="19">
-      <c r="A23" s="41" t="n"/>
-      <c r="B23" s="24" t="n"/>
+      <c r="A23" s="41" t="n">
+        <v>5</v>
+      </c>
+      <c r="B23" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C23" s="25" t="n"/>
       <c r="D23" s="26" t="inlineStr">
         <is>
-          <t>LUCIO</t>
+          <t>MARIE</t>
         </is>
       </c>
       <c r="E23" s="27" t="n"/>
@@ -5892,12 +6044,16 @@
       <c r="BB23" s="33" t="n"/>
     </row>
     <row r="24" ht="13.75" customHeight="1" s="19">
-      <c r="A24" s="41" t="n"/>
-      <c r="B24" s="24" t="n"/>
+      <c r="A24" s="41" t="n">
+        <v>4</v>
+      </c>
+      <c r="B24" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C24" s="25" t="n"/>
       <c r="D24" s="26" t="inlineStr">
         <is>
-          <t>MARIE</t>
+          <t>LUCIO</t>
         </is>
       </c>
       <c r="E24" s="27" t="n"/>
@@ -7865,12 +8021,16 @@
       </c>
     </row>
     <row r="8" ht="13.75" customHeight="1" s="19">
-      <c r="A8" s="41" t="n"/>
-      <c r="B8" s="24" t="n"/>
+      <c r="A8" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C8" s="25" t="n"/>
       <c r="D8" s="26" t="inlineStr">
         <is>
-          <t>IDA</t>
+          <t>H0MBRE 5</t>
         </is>
       </c>
       <c r="E8" s="27" t="n"/>
@@ -7925,12 +8085,16 @@
       <c r="BB8" s="32" t="n"/>
     </row>
     <row r="9" ht="13.75" customHeight="1" s="19">
-      <c r="A9" s="41" t="n"/>
-      <c r="B9" s="24" t="n"/>
+      <c r="A9" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" s="24" t="n">
+        <v>2</v>
+      </c>
       <c r="C9" s="25" t="n"/>
       <c r="D9" s="26" t="inlineStr">
         <is>
-          <t>LOTTE</t>
+          <t>MUJER 3</t>
         </is>
       </c>
       <c r="E9" s="27" t="n"/>
@@ -7985,12 +8149,16 @@
       <c r="BB9" s="33" t="n"/>
     </row>
     <row r="10" ht="13.75" customHeight="1" s="19">
-      <c r="A10" s="41" t="n"/>
-      <c r="B10" s="24" t="n"/>
+      <c r="A10" s="41" t="n">
+        <v>4</v>
+      </c>
+      <c r="B10" s="24" t="n">
+        <v>2</v>
+      </c>
       <c r="C10" s="25" t="n"/>
       <c r="D10" s="26" t="inlineStr">
         <is>
-          <t>ANTON</t>
+          <t>LUCIO</t>
         </is>
       </c>
       <c r="E10" s="27" t="n"/>
@@ -8045,12 +8213,16 @@
       <c r="BB10" s="33" t="n"/>
     </row>
     <row r="11" ht="13.75" customHeight="1" s="19">
-      <c r="A11" s="41" t="n"/>
-      <c r="B11" s="24" t="n"/>
+      <c r="A11" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C11" s="25" t="n"/>
       <c r="D11" s="26" t="inlineStr">
         <is>
-          <t>MUJER 3</t>
+          <t>HOMBRE 6</t>
         </is>
       </c>
       <c r="E11" s="27" t="n"/>
@@ -8105,12 +8277,16 @@
       <c r="BB11" s="33" t="n"/>
     </row>
     <row r="12" ht="13.75" customHeight="1" s="19">
-      <c r="A12" s="41" t="n"/>
-      <c r="B12" s="24" t="n"/>
+      <c r="A12" s="41" t="n">
+        <v>6</v>
+      </c>
+      <c r="B12" s="24" t="n">
+        <v>4</v>
+      </c>
       <c r="C12" s="25" t="n"/>
       <c r="D12" s="26" t="inlineStr">
         <is>
-          <t>HOMBRE 6</t>
+          <t>HERMANN</t>
         </is>
       </c>
       <c r="E12" s="27" t="n"/>
@@ -8165,12 +8341,16 @@
       <c r="BB12" s="33" t="n"/>
     </row>
     <row r="13" ht="13.75" customHeight="1" s="19">
-      <c r="A13" s="41" t="n"/>
-      <c r="B13" s="24" t="n"/>
+      <c r="A13" s="41" t="n">
+        <v>26</v>
+      </c>
+      <c r="B13" s="24" t="n">
+        <v>8</v>
+      </c>
       <c r="C13" s="25" t="n"/>
       <c r="D13" s="26" t="inlineStr">
         <is>
-          <t>HERMANN</t>
+          <t>IDA</t>
         </is>
       </c>
       <c r="E13" s="27" t="n"/>
@@ -8225,12 +8405,16 @@
       <c r="BB13" s="33" t="n"/>
     </row>
     <row r="14" ht="13.75" customHeight="1" s="19">
-      <c r="A14" s="41" t="n"/>
-      <c r="B14" s="24" t="n"/>
+      <c r="A14" s="41" t="n">
+        <v>14</v>
+      </c>
+      <c r="B14" s="24" t="n">
+        <v>4</v>
+      </c>
       <c r="C14" s="25" t="n"/>
       <c r="D14" s="26" t="inlineStr">
         <is>
-          <t>OTTO</t>
+          <t>ANTON</t>
         </is>
       </c>
       <c r="E14" s="27" t="n"/>
@@ -8285,12 +8469,16 @@
       <c r="BB14" s="33" t="n"/>
     </row>
     <row r="15" ht="13.75" customHeight="1" s="19">
-      <c r="A15" s="41" t="n"/>
-      <c r="B15" s="24" t="n"/>
+      <c r="A15" s="41" t="n">
+        <v>6</v>
+      </c>
+      <c r="B15" s="24" t="n">
+        <v>2</v>
+      </c>
       <c r="C15" s="25" t="n"/>
       <c r="D15" s="26" t="inlineStr">
         <is>
-          <t>HOMBRE 4</t>
+          <t>HELENE</t>
         </is>
       </c>
       <c r="E15" s="27" t="n"/>
@@ -8345,12 +8533,16 @@
       <c r="BB15" s="33" t="n"/>
     </row>
     <row r="16" ht="13.75" customHeight="1" s="19">
-      <c r="A16" s="41" t="n"/>
-      <c r="B16" s="24" t="n"/>
+      <c r="A16" s="41" t="n">
+        <v>16</v>
+      </c>
+      <c r="B16" s="24" t="n">
+        <v>6</v>
+      </c>
       <c r="C16" s="25" t="n"/>
       <c r="D16" s="26" t="inlineStr">
         <is>
-          <t>HELENE</t>
+          <t>LOTTE</t>
         </is>
       </c>
       <c r="E16" s="27" t="n"/>
@@ -8405,12 +8597,16 @@
       <c r="BB16" s="33" t="n"/>
     </row>
     <row r="17" ht="13.75" customHeight="1" s="19">
-      <c r="A17" s="41" t="n"/>
-      <c r="B17" s="24" t="n"/>
+      <c r="A17" s="41" t="n">
+        <v>106</v>
+      </c>
+      <c r="B17" s="24" t="n">
+        <v>32</v>
+      </c>
       <c r="C17" s="25" t="n"/>
       <c r="D17" s="26" t="inlineStr">
         <is>
-          <t>INSERTO HANNA</t>
+          <t>HANNA</t>
         </is>
       </c>
       <c r="E17" s="27" t="n"/>
@@ -8465,12 +8661,16 @@
       <c r="BB17" s="33" t="n"/>
     </row>
     <row r="18" ht="13.75" customHeight="1" s="19">
-      <c r="A18" s="41" t="n"/>
-      <c r="B18" s="24" t="n"/>
+      <c r="A18" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="B18" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C18" s="25" t="n"/>
       <c r="D18" s="26" t="inlineStr">
         <is>
-          <t>AMB</t>
+          <t>INSERTO HANNA</t>
         </is>
       </c>
       <c r="E18" s="27" t="n"/>
@@ -8525,12 +8725,16 @@
       <c r="BB18" s="33" t="n"/>
     </row>
     <row r="19" ht="13.75" customHeight="1" s="19">
-      <c r="A19" s="41" t="n"/>
-      <c r="B19" s="24" t="n"/>
+      <c r="A19" s="41" t="n">
+        <v>47</v>
+      </c>
+      <c r="B19" s="24" t="n">
+        <v>13</v>
+      </c>
       <c r="C19" s="25" t="n"/>
       <c r="D19" s="26" t="inlineStr">
         <is>
-          <t>HANNA</t>
+          <t>OTTO</t>
         </is>
       </c>
       <c r="E19" s="27" t="n"/>
@@ -8585,12 +8789,16 @@
       <c r="BB19" s="33" t="n"/>
     </row>
     <row r="20" ht="13.75" customHeight="1" s="19">
-      <c r="A20" s="41" t="n"/>
-      <c r="B20" s="24" t="n"/>
+      <c r="A20" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C20" s="25" t="n"/>
       <c r="D20" s="26" t="inlineStr">
         <is>
-          <t>LUCIO</t>
+          <t>HOMBRE 4</t>
         </is>
       </c>
       <c r="E20" s="27" t="n"/>
@@ -8645,12 +8853,16 @@
       <c r="BB20" s="33" t="n"/>
     </row>
     <row r="21" ht="13.75" customHeight="1" s="19">
-      <c r="A21" s="41" t="n"/>
-      <c r="B21" s="24" t="n"/>
+      <c r="A21" s="41" t="n">
+        <v>28</v>
+      </c>
+      <c r="B21" s="24" t="n">
+        <v>11</v>
+      </c>
       <c r="C21" s="25" t="n"/>
       <c r="D21" s="26" t="inlineStr">
         <is>
-          <t>H0MBRE 5</t>
+          <t>AMB</t>
         </is>
       </c>
       <c r="E21" s="27" t="n"/>
@@ -10786,12 +10998,16 @@
       </c>
     </row>
     <row r="8" ht="13.75" customHeight="1" s="19">
-      <c r="A8" s="41" t="n"/>
-      <c r="B8" s="24" t="n"/>
+      <c r="A8" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" s="24" t="n">
+        <v>2</v>
+      </c>
       <c r="C8" s="25" t="n"/>
       <c r="D8" s="26" t="inlineStr">
         <is>
-          <t>IDA</t>
+          <t>HENRI</t>
         </is>
       </c>
       <c r="E8" s="27" t="n"/>
@@ -10846,12 +11062,16 @@
       <c r="BB8" s="32" t="n"/>
     </row>
     <row r="9" ht="13.75" customHeight="1" s="19">
-      <c r="A9" s="41" t="n"/>
-      <c r="B9" s="24" t="n"/>
+      <c r="A9" s="41" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="24" t="n">
+        <v>6</v>
+      </c>
       <c r="C9" s="25" t="n"/>
       <c r="D9" s="26" t="inlineStr">
         <is>
-          <t>LOTTE</t>
+          <t>INSERTO</t>
         </is>
       </c>
       <c r="E9" s="27" t="n"/>
@@ -10906,12 +11126,16 @@
       <c r="BB9" s="33" t="n"/>
     </row>
     <row r="10" ht="13.75" customHeight="1" s="19">
-      <c r="A10" s="41" t="n"/>
-      <c r="B10" s="24" t="n"/>
+      <c r="A10" s="41" t="n">
+        <v>26</v>
+      </c>
+      <c r="B10" s="24" t="n">
+        <v>2</v>
+      </c>
       <c r="C10" s="25" t="n"/>
       <c r="D10" s="26" t="inlineStr">
         <is>
-          <t>HOMBRE BARCO</t>
+          <t>IDA</t>
         </is>
       </c>
       <c r="E10" s="27" t="n"/>
@@ -10966,8 +11190,12 @@
       <c r="BB10" s="33" t="n"/>
     </row>
     <row r="11" ht="13.75" customHeight="1" s="19">
-      <c r="A11" s="41" t="n"/>
-      <c r="B11" s="24" t="n"/>
+      <c r="A11" s="41" t="n">
+        <v>6</v>
+      </c>
+      <c r="B11" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C11" s="25" t="n"/>
       <c r="D11" s="26" t="inlineStr">
         <is>
@@ -11026,12 +11254,16 @@
       <c r="BB11" s="33" t="n"/>
     </row>
     <row r="12" ht="13.75" customHeight="1" s="19">
-      <c r="A12" s="41" t="n"/>
-      <c r="B12" s="24" t="n"/>
+      <c r="A12" s="41" t="n">
+        <v>16</v>
+      </c>
+      <c r="B12" s="24" t="n">
+        <v>3</v>
+      </c>
       <c r="C12" s="25" t="n"/>
       <c r="D12" s="26" t="inlineStr">
         <is>
-          <t>HENRI</t>
+          <t>LOTTE</t>
         </is>
       </c>
       <c r="E12" s="27" t="n"/>
@@ -11086,12 +11318,16 @@
       <c r="BB12" s="33" t="n"/>
     </row>
     <row r="13" ht="13.75" customHeight="1" s="19">
-      <c r="A13" s="41" t="n"/>
-      <c r="B13" s="24" t="n"/>
+      <c r="A13" s="41" t="n">
+        <v>106</v>
+      </c>
+      <c r="B13" s="24" t="n">
+        <v>6</v>
+      </c>
       <c r="C13" s="25" t="n"/>
       <c r="D13" s="26" t="inlineStr">
         <is>
-          <t>AMB</t>
+          <t>HANNA</t>
         </is>
       </c>
       <c r="E13" s="27" t="n"/>
@@ -11146,12 +11382,16 @@
       <c r="BB13" s="33" t="n"/>
     </row>
     <row r="14" ht="13.75" customHeight="1" s="19">
-      <c r="A14" s="41" t="n"/>
-      <c r="B14" s="24" t="n"/>
+      <c r="A14" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C14" s="25" t="n"/>
       <c r="D14" s="26" t="inlineStr">
         <is>
-          <t>HANNA</t>
+          <t>HOMBRE BARCO</t>
         </is>
       </c>
       <c r="E14" s="27" t="n"/>
@@ -11206,8 +11446,12 @@
       <c r="BB14" s="33" t="n"/>
     </row>
     <row r="15" ht="13.75" customHeight="1" s="19">
-      <c r="A15" s="41" t="n"/>
-      <c r="B15" s="24" t="n"/>
+      <c r="A15" s="41" t="n">
+        <v>5</v>
+      </c>
+      <c r="B15" s="24" t="n">
+        <v>1</v>
+      </c>
       <c r="C15" s="25" t="n"/>
       <c r="D15" s="26" t="inlineStr">
         <is>
@@ -11266,12 +11510,16 @@
       <c r="BB15" s="33" t="n"/>
     </row>
     <row r="16" ht="13.75" customHeight="1" s="19">
-      <c r="A16" s="41" t="n"/>
-      <c r="B16" s="24" t="n"/>
+      <c r="A16" s="41" t="n">
+        <v>28</v>
+      </c>
+      <c r="B16" s="24" t="n">
+        <v>3</v>
+      </c>
       <c r="C16" s="25" t="n"/>
       <c r="D16" s="26" t="inlineStr">
         <is>
-          <t>INSERTO</t>
+          <t>AMB</t>
         </is>
       </c>
       <c r="E16" s="27" t="n"/>

</xml_diff>